<commit_message>
Collected two pilot subjects' data and did some work on organizing the data for the plotting and the analyses.
</commit_message>
<xml_diff>
--- a/analyses/prelim_results.xlsx
+++ b/analyses/prelim_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
   <si>
     <t>1-above_h</t>
   </si>
@@ -86,7 +86,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -130,18 +130,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -471,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -482,7 +490,7 @@
     <col min="2" max="2" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,43 +498,113 @@
         <f>AVERAGE(A2,A4,A6,A8)</f>
         <v>6.2867424242425002E-2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
+        <f>AVERAGE(C2,C4,C6,C8)</f>
+        <v>9.2149038461549981E-2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1">
+        <f>AVERAGE(E2,E4,E6,E8)</f>
+        <v>0.15246527777774999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>7.3636363636399998E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>7.5833333333300001E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4">
+        <v>0.15625</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5.86666666667E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>0.11874999999999999</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6">
+        <v>0.134444444444</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>4.33333333333E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>7.3846153846199997E-2</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8">
+        <v>0.15666666666699999</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -534,43 +612,113 @@
         <f>AVERAGE(A10,A12,A14,A16)</f>
         <v>6.767676767677501E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <f>AVERAGE(C10,C12,C14,C16)</f>
+        <v>9.1023989899000013E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
+        <f>AVERAGE(E10,E12,E14,E16)</f>
+        <v>0.15442361111125003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>6.1818181818200001E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>8.7777777777800006E-2</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <v>0.117777777778</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>7.88888888889E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12">
+        <v>0.116666666667</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>5.7333333333299999E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>9.1818181818200006E-2</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14">
+        <v>0.152</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>7.2666666666700006E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>9.7500000000000003E-2</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16">
+        <v>0.23125000000000001</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -578,43 +726,113 @@
         <f>AVERAGE(A18,A20,A22,A24)</f>
         <v>7.649621212122501E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1">
+        <f>AVERAGE(C18,C20,C22,C24)</f>
+        <v>0.12264330808070001</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1">
+        <f>AVERAGE(E18,E20,E22,E24)</f>
+        <v>0.14784722222225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>8.1818181818199998E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>8.7777777777800006E-2</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18">
+        <v>0.13250000000000001</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>8.2500000000000004E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20">
+        <v>0.142307692308</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>8.1000000000000003E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22">
+        <v>0.15454545454499999</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22">
+        <v>0.12888888888899999</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>6.0666666666700002E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <v>0.15625</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24">
+        <v>0.18769230769199999</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -622,43 +840,113 @@
         <f>AVERAGE(A26,A28,A30,A32)</f>
         <v>7.0232371794875001E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1">
+        <f>AVERAGE(C26,C28,C30,C32)</f>
+        <v>8.8981837606849995E-2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1">
+        <f>AVERAGE(E26,E28,E30,E32)</f>
+        <v>0.12022727272724999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>9.375E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26">
+        <v>8.5555555555600002E-2</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28">
+        <v>8.0833333333300006E-2</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28">
+        <v>0.13090909090899999</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>4.33333333333E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>8.3846153846200006E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32">
+        <v>9.1538461538499996E-2</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32">
+        <v>0.122</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -666,41 +954,111 @@
         <f>AVERAGE(A34,A36,A38,A40)</f>
         <v>7.5645146520124995E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="1">
+        <f>AVERAGE(C34,C36,C38,C40)</f>
+        <v>8.7276515151500006E-2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="1">
+        <f>AVERAGE(E34,E36,E38,E40)</f>
+        <v>9.9020833333324981E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>8.5833333333299996E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>8.4285714285700003E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36">
+        <v>9.0833333333300001E-2</v>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>6.4000000000000001E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38">
+        <v>8.3333333333299994E-2</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38">
+        <v>0.13125000000000001</v>
+      </c>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>6.8461538461499993E-2</v>
       </c>
+      <c r="C40">
+        <v>9.7272727272700005E-2</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="F40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Collected more data. Compiled a DataFrame-based data set and seaborn-based plots for threashold visualization. Further steps will include visualizing threasholds across subjects.
</commit_message>
<xml_diff>
--- a/analyses/prelim_results.xlsx
+++ b/analyses/prelim_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="prelim_aves" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="20">
   <si>
     <t>1-above_h</t>
   </si>
@@ -85,8 +85,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -130,7 +131,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -138,18 +139,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,18 +489,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,21 +530,44 @@
         <f>AVERAGE(E2,E4,E6,E8)</f>
         <v>0.15246527777774999</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1">
+        <f>AVERAGE(G2,G4,G6,G8)</f>
+        <v>0.11604166666675</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1">
+        <f>AVERAGE(I2,I4,I6,I8)</f>
+        <v>0.20887499999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2">
         <v>7.3636363636399998E-2</v>
       </c>
-      <c r="C2">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
         <v>0.16250000000000001</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -538,21 +579,38 @@
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2">
         <v>7.5833333333300001E-2</v>
       </c>
-      <c r="C4">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
         <v>0.15625</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
+        <v>0.1125</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4">
+        <v>0.191666666667</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -564,21 +622,33 @@
         <v>2</v>
       </c>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1">
+      <c r="A6" s="2">
         <v>5.86666666667E-2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.11874999999999999</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>0.134444444444</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -590,21 +660,33 @@
         <v>3</v>
       </c>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
+      <c r="G7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" s="2" customFormat="1">
+      <c r="A8" s="2">
         <v>4.33333333333E-2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>7.3846153846199997E-2</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>0.15666666666699999</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="2">
+        <v>0.106666666667</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.13583333333299999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -626,21 +708,39 @@
         <f>AVERAGE(E10,E12,E14,E16)</f>
         <v>0.15442361111125003</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1">
+        <f>AVERAGE(G10,G12,G14,G16)</f>
+        <v>9.7028499278575001E-2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="1">
+        <f>AVERAGE(I10,I12,I14,I16)</f>
+        <v>0.19015530303025002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1">
+      <c r="A10" s="2">
         <v>6.1818181818200001E-2</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>8.7777777777800006E-2</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>0.117777777778</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="2">
+        <v>7.7272727272700001E-2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -652,21 +752,33 @@
         <v>5</v>
       </c>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" s="2" customFormat="1">
+      <c r="A12" s="2">
         <v>7.88888888889E-2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>0.116666666667</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="2">
+        <v>0.119285714286</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.17333333333299999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -678,21 +790,33 @@
         <v>6</v>
       </c>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" s="2" customFormat="1">
+      <c r="A14" s="2">
         <v>5.7333333333299999E-2</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>9.1818181818200006E-2</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>0.152</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="2">
+        <v>0.106</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.215833333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -704,21 +828,33 @@
         <v>7</v>
       </c>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" s="2" customFormat="1">
+      <c r="A16" s="2">
         <v>7.2666666666700006E-2</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>9.7500000000000003E-2</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>0.23125000000000001</v>
       </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="2">
+        <v>8.5555555555600002E-2</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.15545454545500001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -740,21 +876,39 @@
         <f>AVERAGE(E18,E20,E22,E24)</f>
         <v>0.14784722222225</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18">
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="1">
+        <f>AVERAGE(G18,G20,G22,G24)</f>
+        <v>8.4499999999999992E-2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="1">
+        <f>AVERAGE(I18,I20,I22,I24)</f>
+        <v>0.1800208333335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="2" customFormat="1">
+      <c r="A18" s="2">
         <v>8.1818181818199998E-2</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>8.7777777777800006E-2</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>0.13250000000000001</v>
       </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.23125000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -766,21 +920,33 @@
         <v>9</v>
       </c>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20">
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" s="2" customFormat="1">
+      <c r="A20" s="2">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>0.142307692308</v>
       </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.25800000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -792,21 +958,33 @@
         <v>10</v>
       </c>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22">
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" s="2" customFormat="1">
+      <c r="A22" s="2">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>0.15454545454499999</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>0.12888888888899999</v>
       </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.12416666666700001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -818,21 +996,33 @@
         <v>11</v>
       </c>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24">
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" s="2" customFormat="1">
+      <c r="A24" s="2">
         <v>6.0666666666700002E-2</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>0.15625</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>0.18769230769199999</v>
       </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="2">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.106666666667</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -854,21 +1044,39 @@
         <f>AVERAGE(E26,E28,E30,E32)</f>
         <v>0.12022727272724999</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26">
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="1">
+        <f>AVERAGE(G26,G28,G30,G32)</f>
+        <v>9.3688672438725001E-2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="1">
+        <f>AVERAGE(I26,I28,I30,I32)</f>
+        <v>0.1639903846155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="2" customFormat="1">
+      <c r="A26" s="2">
         <v>9.375E-2</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>8.5555555555600002E-2</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" s="2">
+        <v>8.1818181818199998E-2</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -880,21 +1088,33 @@
         <v>13</v>
       </c>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28">
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" s="2" customFormat="1">
+      <c r="A28" s="2">
         <v>0.06</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>8.0833333333300006E-2</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>0.13090909090899999</v>
       </c>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" s="2">
+        <v>9.07142857143E-2</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0.19846153846199999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -906,21 +1126,33 @@
         <v>14</v>
       </c>
       <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30">
+      <c r="G29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" s="2" customFormat="1">
+      <c r="A30" s="2">
         <v>4.33333333333E-2</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>0.14099999999999999</v>
       </c>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="2">
+        <v>8.4444444444399996E-2</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -932,21 +1164,33 @@
         <v>15</v>
       </c>
       <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32">
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" s="2" customFormat="1">
+      <c r="A32" s="2">
         <v>8.3846153846200006E-2</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>9.1538461538499996E-2</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>0.122</v>
       </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" s="2">
+        <v>0.117777777778</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0.1125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -968,21 +1212,39 @@
         <f>AVERAGE(E34,E36,E38,E40)</f>
         <v>9.9020833333324981E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34">
+      <c r="G33" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="1">
+        <f>AVERAGE(G34,G36,G38,G40)</f>
+        <v>8.6565656565650004E-2</v>
+      </c>
+      <c r="I33" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="1">
+        <f>AVERAGE(I34,I36,I38,I40)</f>
+        <v>0.11395833333345</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="2" customFormat="1">
+      <c r="A34" s="2">
         <v>8.5833333333299996E-2</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34" s="2">
+        <v>8.1818181818199998E-2</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0.1125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -994,21 +1256,33 @@
         <v>17</v>
       </c>
       <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36">
+      <c r="G35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" s="2" customFormat="1">
+      <c r="A36" s="2">
         <v>8.4285714285700003E-2</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>9.0833333333300001E-2</v>
       </c>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0.15555555555600001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -1020,21 +1294,33 @@
         <v>18</v>
       </c>
       <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38">
+      <c r="G37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" s="2" customFormat="1">
+      <c r="A38" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="2">
         <v>8.3333333333299994E-2</v>
       </c>
-      <c r="D38" s="1"/>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>0.13125000000000001</v>
       </c>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38" s="2">
+        <v>9.1111111111099999E-2</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1046,19 +1332,31 @@
         <v>19</v>
       </c>
       <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40">
+      <c r="G39" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" s="2" customFormat="1">
+      <c r="A40" s="2">
         <v>6.8461538461499993E-2</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <v>9.7272727272700005E-2</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="G40" s="2">
+        <v>8.3333333333299994E-2</v>
+      </c>
+      <c r="I40" s="2">
+        <v>8.7777777777800006E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>